<commit_message>
Issue #18: added support for files with different encoding
</commit_message>
<xml_diff>
--- a/src/app/shared/services/reader/excel/test.xlsx
+++ b/src/app/shared/services/reader/excel/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspaces.git\koia\src\app\shared\services\reader\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace.koia\koia\src\app\shared\services\reader\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -367,7 +367,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,7 +414,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="1">
-        <v>43621</v>
+        <v>43622</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>